<commit_message>
Added refactorings for 4.1.1
</commit_message>
<xml_diff>
--- a/doc/refactoring-4.0.x-to-4.1.0/Refactorings 4.0.x to 4.1.0.xlsx
+++ b/doc/refactoring-4.0.x-to-4.1.0/Refactorings 4.0.x to 4.1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-4.1.x-to-5.0.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-4.0.x-to-4.1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EC3184-F060-CE4D-9CCE-88039A683231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D60DF-ED05-B24A-8D8F-224F3E561E07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>interface</t>
   </si>
@@ -107,9 +107,6 @@
     <t>4.0.x</t>
   </si>
   <si>
-    <t>4.1.x</t>
-  </si>
-  <si>
     <t>SwaptionATMMarketDataFromArray</t>
   </si>
   <si>
@@ -117,6 +114,18 @@
   </si>
   <si>
     <t>ProcessWithFactorDrift</t>
+  </si>
+  <si>
+    <t>RandomVariableDifferentiableFactory</t>
+  </si>
+  <si>
+    <t>AbstractRandomVariableDifferentiableFactory</t>
+  </si>
+  <si>
+    <t>(extracted interface) since 4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
   </si>
 </sst>
 </file>
@@ -210,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -221,6 +230,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -535,11 +545,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -558,8 +566,8 @@
       <c r="C1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>25</v>
+      <c r="D1" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>6</v>
@@ -611,7 +619,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>1</v>
@@ -669,7 +677,7 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>0</v>
@@ -685,7 +693,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
         <v>1</v>
@@ -725,7 +733,28 @@
       </c>
       <c r="F17" s="4"/>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="D1" twoDigitTextYear="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>